<commit_message>
Added writing into .xlsx logic
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/ExpressRegistrationTestdata1.xlsx
+++ b/src/main/java/com/testdata/ExpressRegistrationTestdata1.xlsx
@@ -194,12 +194,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>